<commit_message>
1) openpyexcel was replaced with pandas 2) word counters was added
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="settings" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="875771161" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="settings" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="875771161" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -429,13 +429,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="C1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="10" bestFit="1" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="C1" t="inlineStr">
@@ -445,7 +448,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>2015_2014_2013_2012_1821_2008_ 2007_ 2006_ 2005_ 2004_318_2002_235_1999_1998_1997</t>
+          <t>2032_2030_2029_2028_2026_2025</t>
         </is>
       </c>
     </row>
@@ -460,32 +463,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
           <t>&lt;-pack's name</t>
         </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>parser:</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -506,100 +501,130 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="1" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
-      <c r="C4" s="1" t="n"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
-      <c r="C5" s="1" t="n"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
-      <c r="C6" s="1" t="n"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
-      <c r="C7" s="1" t="n"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
-      <c r="C8" s="1" t="n"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
-      <c r="C9" s="1" t="n"/>
-    </row>
-    <row r="10">
-      <c r="C10" s="1" t="n"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="1" t="n"/>
-    </row>
-    <row r="12">
-      <c r="C12" s="1" t="n"/>
-    </row>
-    <row r="13">
-      <c r="C13" s="1" t="n"/>
-    </row>
-    <row r="14">
-      <c r="C14" s="1" t="n"/>
-    </row>
-    <row r="15">
-      <c r="C15" s="1" t="n"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="1" t="n"/>
-    </row>
-    <row r="17">
-      <c r="C17" s="1" t="n"/>
-    </row>
-    <row r="18">
-      <c r="C18" s="1" t="n"/>
-    </row>
-    <row r="19">
-      <c r="C19" s="1" t="n"/>
-    </row>
-    <row r="20">
-      <c r="C20" s="1" t="n"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="1" t="n"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="1" t="n"/>
-    </row>
-    <row r="23">
-      <c r="C23" s="1" t="n"/>
-    </row>
-    <row r="24">
-      <c r="C24" s="1" t="n"/>
-    </row>
-    <row r="25">
-      <c r="C25" s="1" t="n"/>
-    </row>
-    <row r="26">
-      <c r="C26" s="1" t="n"/>
-    </row>
-    <row r="27">
-      <c r="C27" s="1" t="n"/>
-    </row>
-    <row r="28">
-      <c r="C28" s="1" t="n"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="1" t="n"/>
-    </row>
-    <row r="30">
-      <c r="C30" s="1" t="n"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="1" t="n"/>
-    </row>
-    <row r="32">
-      <c r="C32" s="1" t="n"/>
-    </row>
-    <row r="33">
-      <c r="C33" s="1" t="n"/>
-    </row>
-    <row r="34">
-      <c r="C34" s="1" t="n"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>45592</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>